<commit_message>
Moved videos and added Hat BOMs
Moved Tutorial videos and added BOMs for hat switches
</commit_message>
<xml_diff>
--- a/Documentation/BOMs/Wilson Thrust BOM v4 Cheaper with Grip LEDs.xlsx
+++ b/Documentation/BOMs/Wilson Thrust BOM v4 Cheaper with Grip LEDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7a43267b7fa0998/Github Repositories/WilsonThrust510/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7a43267b7fa0998/Github Repositories/WilsonThrust510/Documentation/BOMs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95FFF89C-6BD3-4AA2-B911-7DB1035EFB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{95FFF89C-6BD3-4AA2-B911-7DB1035EFB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA825937-054F-40F7-BD0C-263B32EE8B82}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{C99EEBEB-5120-4843-8B17-4416EAFBA3F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{C99EEBEB-5120-4843-8B17-4416EAFBA3F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Large PCB Parts" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="393">
   <si>
     <t>Amazon</t>
   </si>
@@ -256,19 +256,6 @@
   </si>
   <si>
     <t>Springs</t>
-  </si>
-  <si>
-    <t>3HPC7</t>
-  </si>
-  <si>
-    <t>3HPG3</t>
-  </si>
-  <si>
-    <t>Used for the following part:
-Detent Pullup Grip</t>
-  </si>
-  <si>
-    <t>Zoro</t>
   </si>
   <si>
     <t>Screw Pin</t>
@@ -431,10 +418,6 @@
   </si>
   <si>
     <t xml:space="preserve">Only needed if not mounting.  Otherwise, pick the shape, size, color, and brand you like.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can pick a different tension springs if you'd like.  These are 1.071 lb at halfway up the leg extension which is quite heavy.  If you go lighter or heavier, you just want to make sure it's not too much wider (Wire Diameter x Number of Coils) and that it has a Max. Rod Outside Diameter of 0.187 in or larger. Also, know that you'll need one wind direction left hand and one right hand.
 </t>
   </si>
   <si>
@@ -4586,112 +4569,9 @@
 </t>
   </si>
   <si>
-    <r>
-      <t>Catagory:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Torsion Spring</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Spring Length @ Torque: 0.625 in
-Deflection Angle (Deg.): 90
-Leg Length: 1.25 in
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Max. Rod Outside Dia.: 0.187 in
-Wind Direction: Left Hand
-Wire Dia.: 0.035 in
-Outside Dia.: 0.315 in
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Used for the following part:
 Detent Pullup Grip
 </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Catagory: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Torsion Spring</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Spring Length @ Torque: 0.625 in
-Deflection Angle (Deg.): 90
-Leg Length: 1.25 in
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Max. Rod Outside Dia.: 0.187 in
-Wind Direction: Right Hand
-Wire Dia.: 0.035 in
-Outside Dia.: 0.315 in
-</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Torque @ 1/2 Leg Length (In.-Lbs.): 1.071
-Number of Coils: 3.25
-Lot: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6 pcs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
   </si>
   <si>
     <r>
@@ -5132,6 +5012,102 @@
     <t xml:space="preserve">So, you can get the cheaper Uxcell bearings which are 13.45 for 10 (and only use 3) or you can get nicer bearings.  It's up to you.  Just know there is a difference.  Here is a link to the bearings I ended up using from McMaster-Carr: https://www.mcmaster.com/5972K279/
 The McMaster-Carr bearings are smoother than any bearing I've gotten from amazon but you pay much more for that quality and precision.
 </t>
+  </si>
+  <si>
+    <r>
+      <t>Catagory:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Extension Spring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Length: 0.875 in.
+OD: 0.24 in.
+Wire Diameter: 0.022 in.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Extended Length @ Maximum Load: 2 in.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Load, lbs.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Min.: .16
+Max: 1.72</t>
+    </r>
+  </si>
+  <si>
+    <t>7749N106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can pick a different extension springs if you'd like.  If you go lighter or heavier, you just want to make sure it's length is close to 0.875 inches and the loops are around 0.24 inches.
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spring Rating: 1.416 lbs./in.
+Material: 302 Stainless Steel
+End Type: Loop
+Lot: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5 pcs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -5366,7 +5342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -5389,30 +5365,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -5424,53 +5386,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -5478,20 +5395,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5549,6 +5457,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5878,7 +5789,7 @@
     <col min="2" max="2" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="65.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -5887,50 +5798,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>361</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>391</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>362</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>363</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>364</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>365</v>
-      </c>
-      <c r="I1" s="38" t="s">
+      <c r="A1" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="38" t="s">
-        <v>158</v>
+      <c r="J1" s="17" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="59"/>
+      <c r="A2" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -5940,16 +5851,16 @@
         <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>100</v>
+        <v>139</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>0</v>
@@ -5957,7 +5868,7 @@
       <c r="H3" s="4">
         <v>6.99</v>
       </c>
-      <c r="I3" s="34"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -5967,16 +5878,16 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>95</v>
+        <v>90</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>3</v>
@@ -5984,23 +5895,23 @@
       <c r="H4" s="4">
         <v>0.04</v>
       </c>
-      <c r="I4" s="34" t="s">
-        <v>145</v>
+      <c r="I4" s="6" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="55"/>
+      <c r="A5" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
     </row>
     <row r="6" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -6010,16 +5921,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>234</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>146</v>
+        <v>92</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>3</v>
@@ -6027,21 +5938,21 @@
       <c r="H6" s="4">
         <v>0.35</v>
       </c>
-      <c r="I6" s="34"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="55"/>
+      <c r="A7" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="31"/>
     </row>
     <row r="8" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -6053,13 +5964,13 @@
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="F8" s="28" t="s">
+      <c r="D8" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -6068,21 +5979,21 @@
       <c r="H8" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="I8" s="34"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="55"/>
+      <c r="A9" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
     </row>
     <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -6092,16 +6003,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>93</v>
+        <v>142</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>0</v>
@@ -6109,21 +6020,21 @@
       <c r="H10" s="5">
         <v>18.53</v>
       </c>
-      <c r="I10" s="34"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="55"/>
+      <c r="A11" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="31"/>
     </row>
     <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -6132,14 +6043,14 @@
       <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>149</v>
+      <c r="D12" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>1</v>
@@ -6147,11 +6058,11 @@
       <c r="H12" s="5">
         <v>1.65</v>
       </c>
-      <c r="I12" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="J12" s="56" t="s">
-        <v>108</v>
+      <c r="I12" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -6161,14 +6072,14 @@
       <c r="B13" s="1">
         <v>24</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>153</v>
+      <c r="D13" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>1</v>
@@ -6176,10 +6087,10 @@
       <c r="H13" s="5">
         <v>4.6900000000000004</v>
       </c>
-      <c r="I13" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="J13" s="56"/>
+      <c r="I13" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" s="32"/>
     </row>
     <row r="14" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -6188,14 +6099,14 @@
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>150</v>
+      <c r="C14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>1</v>
@@ -6203,10 +6114,10 @@
       <c r="H14" s="5">
         <v>2.0499999999999998</v>
       </c>
-      <c r="I14" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="J14" s="56"/>
+      <c r="I14" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -6215,14 +6126,14 @@
       <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>151</v>
+      <c r="D15" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>1</v>
@@ -6230,10 +6141,10 @@
       <c r="H15" s="5">
         <v>1.96</v>
       </c>
-      <c r="I15" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="J15" s="56"/>
+      <c r="I15" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -6242,14 +6153,14 @@
       <c r="B16" s="1">
         <v>5</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>152</v>
+      <c r="D16" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>1</v>
@@ -6257,24 +6168,24 @@
       <c r="H16" s="5">
         <v>6.64</v>
       </c>
-      <c r="I16" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="J16" s="56"/>
+      <c r="I16" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J16" s="32"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="55"/>
+      <c r="A17" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -6286,13 +6197,13 @@
       <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="F18" s="28" t="s">
+      <c r="D18" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -6310,15 +6221,15 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E19" s="33" t="s">
-        <v>232</v>
-      </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -6338,13 +6249,13 @@
       <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="F20" s="28" t="s">
+      <c r="D20" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -6353,8 +6264,8 @@
       <c r="H20" s="4">
         <v>10.97</v>
       </c>
-      <c r="I20" s="34" t="s">
-        <v>159</v>
+      <c r="I20" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -6402,7 +6313,7 @@
     <col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46.140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="4" bestFit="1" customWidth="1"/>
@@ -6410,31 +6321,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>361</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>391</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>362</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>363</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>364</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>365</v>
-      </c>
-      <c r="I1" s="38" t="s">
+      <c r="A1" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6449,13 +6360,13 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>212</v>
+        <v>211</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>3</v>
@@ -6463,8 +6374,8 @@
       <c r="H2" s="4">
         <v>0.28399999999999997</v>
       </c>
-      <c r="I2" s="34" t="s">
-        <v>143</v>
+      <c r="I2" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -6478,13 +6389,13 @@
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>213</v>
+        <v>210</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>3</v>
@@ -6492,8 +6403,8 @@
       <c r="H3" s="5">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="I3" s="34" t="s">
-        <v>141</v>
+      <c r="I3" s="6" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -6507,13 +6418,13 @@
         <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>217</v>
+        <v>209</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>3</v>
@@ -6521,8 +6432,8 @@
       <c r="H4" s="5">
         <v>0.125</v>
       </c>
-      <c r="I4" s="34" t="s">
-        <v>142</v>
+      <c r="I4" s="6" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6585,8 +6496,8 @@
     <col min="2" max="2" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="4" bestFit="1" customWidth="1"/>
@@ -6595,50 +6506,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>361</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>391</v>
-      </c>
-      <c r="C1" s="50" t="s">
-        <v>362</v>
-      </c>
-      <c r="D1" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>160</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>363</v>
-      </c>
-      <c r="H1" s="50" t="s">
-        <v>364</v>
-      </c>
-      <c r="I1" s="50" t="s">
-        <v>365</v>
-      </c>
-      <c r="J1" s="50" t="s">
+      <c r="A1" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -6647,17 +6558,17 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>139</v>
+      <c r="C3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>0</v>
@@ -6665,8 +6576,8 @@
       <c r="I3" s="5">
         <v>13.69</v>
       </c>
-      <c r="J3" s="32" t="s">
-        <v>114</v>
+      <c r="J3" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -6680,16 +6591,16 @@
         <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>185</v>
+        <v>179</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>3</v>
@@ -6709,16 +6620,16 @@
         <v>67</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>385</v>
+        <v>376</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>5</v>
@@ -6729,18 +6640,18 @@
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
     </row>
     <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -6753,16 +6664,16 @@
         <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>188</v>
+        <v>380</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>5</v>
@@ -6783,16 +6694,16 @@
         <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>190</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>191</v>
+        <v>184</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>5</v>
@@ -6803,18 +6714,18 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="55"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
     </row>
     <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -6827,16 +6738,16 @@
         <v>68</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>193</v>
+        <v>189</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>3</v>
@@ -6847,18 +6758,18 @@
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="55"/>
+      <c r="A11" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="31"/>
     </row>
     <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -6867,20 +6778,20 @@
       <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>136</v>
+      <c r="C12" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>197</v>
+        <v>190</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>0</v>
@@ -6897,20 +6808,20 @@
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>381</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>372</v>
+      <c r="C13" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>362</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>0</v>
@@ -6918,21 +6829,21 @@
       <c r="I13" s="5">
         <v>10.89</v>
       </c>
-      <c r="J13" s="24"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="31"/>
     </row>
     <row r="15" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -6945,16 +6856,16 @@
         <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E15" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>374</v>
+        <v>194</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>364</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>5</v>
@@ -6965,18 +6876,18 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="55"/>
+      <c r="A16" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="31"/>
     </row>
     <row r="17" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -6989,16 +6900,16 @@
         <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="F17" s="35" t="s">
-        <v>201</v>
+        <v>198</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>5</v>
@@ -7006,7 +6917,7 @@
       <c r="I17" s="4">
         <v>9.61</v>
       </c>
-      <c r="J17" s="56" t="s">
+      <c r="J17" s="32" t="s">
         <v>29</v>
       </c>
     </row>
@@ -7021,16 +6932,16 @@
         <v>27</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="F18" s="35" t="s">
-        <v>179</v>
+        <v>175</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>3</v>
@@ -7038,7 +6949,7 @@
       <c r="I18" s="4">
         <v>14.62</v>
       </c>
-      <c r="J18" s="56"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -7051,16 +6962,16 @@
         <v>28</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>379</v>
-      </c>
-      <c r="F19" s="35" t="s">
-        <v>205</v>
+        <v>199</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>3</v>
@@ -7069,7 +6980,7 @@
         <v>2.3199999999999998</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -7082,14 +6993,14 @@
       <c r="C20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>140</v>
+      <c r="D20" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>31</v>
@@ -7097,23 +7008,23 @@
       <c r="I20" s="4">
         <v>5.5</v>
       </c>
-      <c r="J20" s="22" t="s">
-        <v>377</v>
+      <c r="J20" s="6" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="55"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="31"/>
     </row>
     <row r="22" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -7126,16 +7037,16 @@
         <v>33</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="F22" s="35" t="s">
-        <v>169</v>
+        <v>173</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>3</v>
@@ -7144,22 +7055,22 @@
         <v>20</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="55"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -7172,16 +7083,16 @@
         <v>35</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="F24" s="35" t="s">
-        <v>207</v>
+        <v>203</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>5</v>
@@ -7190,7 +7101,7 @@
         <v>6.04</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -7204,16 +7115,16 @@
         <v>36</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>172</v>
+        <v>166</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>3</v>
@@ -7234,16 +7145,16 @@
         <v>37</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E26" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="F26" s="35" t="s">
-        <v>176</v>
+        <v>169</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>3</v>
@@ -7252,22 +7163,22 @@
         <v>10.09</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="55"/>
+      <c r="A27" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -7277,19 +7188,19 @@
         <v>2</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="F28" s="35" t="s">
-        <v>170</v>
-      </c>
-      <c r="G28" s="23" t="s">
-        <v>387</v>
+        <v>86</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>377</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>3</v>
@@ -7297,8 +7208,8 @@
       <c r="I28" s="5">
         <v>2.4900000000000002</v>
       </c>
-      <c r="J28" s="36" t="s">
-        <v>211</v>
+      <c r="J28" s="6" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -7398,11 +7309,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{686073A0-D06A-4A43-B3C7-39882209510A}">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7411,8 +7322,8 @@
     <col min="2" max="2" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -7421,852 +7332,824 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>361</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>391</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>362</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>363</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>364</v>
-      </c>
-      <c r="I1" s="38" t="s">
-        <v>365</v>
-      </c>
-      <c r="J1" s="38" t="s">
+      <c r="A1" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="38" t="s">
-        <v>158</v>
+      <c r="K1" s="17" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="62"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="52">
+      <c r="A3" s="28">
         <v>8</v>
       </c>
-      <c r="B3" s="52">
+      <c r="B3" s="28">
         <v>8</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="31"/>
+    </row>
+    <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="28">
+        <v>1</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E5" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F3" s="41" t="s">
-        <v>301</v>
-      </c>
-      <c r="G3" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="H3" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="J3" s="47" t="s">
-        <v>297</v>
-      </c>
-      <c r="K3" s="44" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="55"/>
-    </row>
-    <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="52">
-        <v>1</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>392</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>302</v>
-      </c>
-      <c r="F5" s="42" t="s">
-        <v>304</v>
-      </c>
-      <c r="G5" s="42" t="s">
-        <v>115</v>
+      <c r="G5" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="48">
+      <c r="I5" s="24">
         <v>8.99</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="55"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="31"/>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="52">
+      <c r="A7" s="28">
         <v>1</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>392</v>
+      <c r="B7" s="28" t="s">
+        <v>382</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>306</v>
-      </c>
-      <c r="F7" s="42" t="s">
-        <v>307</v>
-      </c>
-      <c r="G7" s="42" t="s">
-        <v>121</v>
+        <v>300</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="48">
+      <c r="I7" s="24">
         <v>14.55</v>
       </c>
-      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="55"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="31"/>
     </row>
     <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="52">
+      <c r="A9" s="28">
         <v>1</v>
       </c>
-      <c r="B9" s="52" t="s">
-        <v>392</v>
+      <c r="B9" s="28" t="s">
+        <v>382</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>311</v>
-      </c>
-      <c r="F9" s="42" t="s">
-        <v>308</v>
-      </c>
-      <c r="G9" s="42" t="s">
-        <v>359</v>
+        <v>305</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="12">
         <v>9.9700000000000006</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="55"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52">
+      <c r="A11" s="28">
         <v>1</v>
       </c>
-      <c r="B11" s="52">
+      <c r="B11" s="28">
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>313</v>
-      </c>
-      <c r="F11" s="42" t="s">
-        <v>314</v>
+        <v>307</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="12">
         <v>7.99</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="K11" s="43" t="s">
-        <v>366</v>
+        <v>357</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="55"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="31"/>
     </row>
     <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="52">
+      <c r="A13" s="28">
         <v>1</v>
       </c>
-      <c r="B13" s="52">
+      <c r="B13" s="28">
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="F13" s="42" t="s">
-        <v>163</v>
+        <v>310</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="12">
         <v>9.99</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="K13" s="43"/>
+        <v>115</v>
+      </c>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="55"/>
-    </row>
-    <row r="15" spans="1:11" s="20" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="40">
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
         <v>1</v>
       </c>
-      <c r="B15" s="40">
+      <c r="B15" s="18">
         <v>3</v>
       </c>
-      <c r="C15" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>317</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>318</v>
-      </c>
-      <c r="F15" s="42" t="s">
+      <c r="C15" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="25">
+        <v>13.49</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="31"/>
+    </row>
+    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="28">
+        <v>1</v>
+      </c>
+      <c r="B17" s="28">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="G15" s="42" t="s">
-        <v>396</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" s="49">
-        <v>13.49</v>
-      </c>
-      <c r="J15" s="43" t="s">
-        <v>397</v>
-      </c>
-      <c r="K15" s="43"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="55"/>
-    </row>
-    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="52">
-        <v>1</v>
-      </c>
-      <c r="B17" s="52">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>329</v>
-      </c>
-      <c r="F17" s="42" t="s">
-        <v>324</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>325</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="12">
         <v>8.3000000000000007</v>
       </c>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="52">
+      <c r="A18" s="28">
         <v>1</v>
       </c>
-      <c r="B18" s="52">
+      <c r="B18" s="28">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>322</v>
-      </c>
-      <c r="F18" s="42" t="s">
-        <v>323</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>326</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="12">
         <v>7.99</v>
       </c>
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="55"/>
+      <c r="A19" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="31"/>
     </row>
     <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="52">
+      <c r="A20" s="28">
         <v>1</v>
       </c>
-      <c r="B20" s="52">
+      <c r="B20" s="28">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>333</v>
-      </c>
-      <c r="F20" s="42" t="s">
         <v>327</v>
       </c>
+      <c r="E20" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>322</v>
+      </c>
       <c r="G20" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="12">
         <v>11.99</v>
       </c>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="52">
+      <c r="A21" s="28">
         <v>1</v>
       </c>
-      <c r="B21" s="52">
+      <c r="B21" s="28">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>331</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>333</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>327</v>
+        <v>122</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I21" s="12">
         <v>12.49</v>
       </c>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="52">
+      <c r="A22" s="28">
         <v>1</v>
       </c>
-      <c r="B22" s="52">
+      <c r="B22" s="28">
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>334</v>
-      </c>
-      <c r="F22" s="42" t="s">
-        <v>328</v>
+        <v>325</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>323</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I22" s="12">
         <v>7.99</v>
       </c>
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="55"/>
+      <c r="A23" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="31"/>
     </row>
     <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="52">
+      <c r="A24" s="28">
         <v>1</v>
       </c>
-      <c r="B24" s="52">
+      <c r="B24" s="28">
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>336</v>
-      </c>
-      <c r="F24" s="42" t="s">
-        <v>358</v>
+        <v>330</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>348</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I24" s="18">
+      <c r="I24" s="12">
         <v>8.99</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="55"/>
+      <c r="A25" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="31"/>
     </row>
     <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="52">
+      <c r="A26" s="28">
         <v>1</v>
       </c>
-      <c r="B26" s="52">
+      <c r="B26" s="28">
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I26" s="12">
+        <v>1.32</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="K26" s="23" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="31"/>
+    </row>
+    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="28">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="E26" s="33" t="s">
-        <v>339</v>
-      </c>
-      <c r="F26" s="42" t="s">
-        <v>338</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="I26" s="18">
-        <v>1.32</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="K26" s="47" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="55"/>
-    </row>
-    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="52">
-        <v>1</v>
-      </c>
-      <c r="B28" s="52">
-        <v>2</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>341</v>
-      </c>
-      <c r="F28" s="42" t="s">
-        <v>349</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>342</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I28" s="18">
+      <c r="I28" s="12">
         <v>5.99</v>
       </c>
       <c r="J28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="55"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="31"/>
     </row>
     <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="52">
+      <c r="A30" s="28">
         <v>1</v>
       </c>
-      <c r="B30" s="52">
+      <c r="B30" s="28">
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>390</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" s="12">
+        <v>16.32</v>
+      </c>
+      <c r="J30" s="39" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="31"/>
+    </row>
+    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="28">
+        <v>1</v>
+      </c>
+      <c r="B32" s="28">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="E30" s="33" t="s">
-        <v>344</v>
-      </c>
-      <c r="F30" s="42" t="s">
-        <v>348</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I30" s="18">
-        <v>4.55</v>
-      </c>
-      <c r="J30" s="56" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="52">
-        <v>1</v>
-      </c>
-      <c r="B31" s="52">
-        <v>1</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="E31" s="33" t="s">
-        <v>347</v>
-      </c>
-      <c r="F31" s="42" t="s">
-        <v>348</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I31" s="18">
-        <v>5.17</v>
-      </c>
-      <c r="J31" s="56"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="53" t="s">
-        <v>98</v>
-      </c>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="54"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="55"/>
-    </row>
-    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="52">
-        <v>1</v>
-      </c>
-      <c r="B33" s="52">
-        <v>4</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>351</v>
-      </c>
-      <c r="E33" s="33" t="s">
+      <c r="G32" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="12">
+        <v>8.99</v>
+      </c>
+      <c r="J32" s="23" t="s">
         <v>350</v>
       </c>
-      <c r="F33" s="42" t="s">
-        <v>353</v>
-      </c>
-      <c r="G33" s="27" t="s">
-        <v>352</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I33" s="18">
-        <v>8.99</v>
-      </c>
-      <c r="J33" s="47" t="s">
-        <v>360</v>
-      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="31"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="55"/>
+      <c r="A34" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34" s="6"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>63</v>
-      </c>
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -8329,27 +8212,23 @@
     <row r="55" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J55" s="6"/>
     </row>
-    <row r="56" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J56" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="A29:K29"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="J30:J31"/>
+  <mergeCells count="15">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A10:K10"/>
     <mergeCell ref="A12:K12"/>
     <mergeCell ref="A14:K14"/>
     <mergeCell ref="A16:K16"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A29:K29"/>
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="A33:K33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1" xr:uid="{EF6854EA-9FC9-4FFA-B284-7464CDC602EE}"/>
@@ -8360,19 +8239,18 @@
     <hyperlink ref="H15" r:id="rId6" xr:uid="{32682F16-4F4F-428E-9C02-7D1F0B67B9AF}"/>
     <hyperlink ref="H3" r:id="rId7" xr:uid="{9C7E491B-4188-438D-AF00-DEFC44C74898}"/>
     <hyperlink ref="H18" r:id="rId8" xr:uid="{8199EDF6-B1ED-4FB9-BD77-B9BF33F28968}"/>
-    <hyperlink ref="H31" r:id="rId9" xr:uid="{8BD9B7BD-11F9-4180-A94E-DC36EA883CB1}"/>
-    <hyperlink ref="H30" r:id="rId10" xr:uid="{3F333B03-3E85-41B7-8AA9-18DC9DE4D965}"/>
-    <hyperlink ref="H28" r:id="rId11" xr:uid="{71D4D980-2A12-4F6C-A297-1013F776DA79}"/>
-    <hyperlink ref="H17" r:id="rId12" xr:uid="{2BCF9FEE-4678-4F55-A819-842E3221F1B8}"/>
-    <hyperlink ref="H20" r:id="rId13" xr:uid="{CE798603-ADF1-46B7-AFA0-781B06FB2CCF}"/>
-    <hyperlink ref="H24" r:id="rId14" xr:uid="{5ECC50D4-780E-4814-B4BC-D4B4C339E08B}"/>
-    <hyperlink ref="H22" r:id="rId15" xr:uid="{1F9C4842-7E2D-40E4-8810-9F7B34D54D76}"/>
-    <hyperlink ref="H26" r:id="rId16" location="Werkstoff%3Du(85eb5967-f719-44cc-a7f3-84339b5839ac)%3Bd1%3Dc(25)%3Bd3%3Du(0c49c7b3-a2d5-4127-b6ac-792d414b1606)%3BForm%3Du(c0aa885f-8ea8-4010-abd2-06a95d4f35f0)" xr:uid="{D6B2EA74-8003-4424-A06E-78E36D093C76}"/>
-    <hyperlink ref="H33" r:id="rId17" xr:uid="{53E8A669-3EB3-4259-A86D-EAE251CED179}"/>
-    <hyperlink ref="H21" r:id="rId18" xr:uid="{C24409C7-1B7A-4386-B792-63EA1927E97A}"/>
+    <hyperlink ref="H30" r:id="rId9" xr:uid="{3F333B03-3E85-41B7-8AA9-18DC9DE4D965}"/>
+    <hyperlink ref="H28" r:id="rId10" xr:uid="{71D4D980-2A12-4F6C-A297-1013F776DA79}"/>
+    <hyperlink ref="H17" r:id="rId11" xr:uid="{2BCF9FEE-4678-4F55-A819-842E3221F1B8}"/>
+    <hyperlink ref="H20" r:id="rId12" xr:uid="{CE798603-ADF1-46B7-AFA0-781B06FB2CCF}"/>
+    <hyperlink ref="H24" r:id="rId13" xr:uid="{5ECC50D4-780E-4814-B4BC-D4B4C339E08B}"/>
+    <hyperlink ref="H22" r:id="rId14" xr:uid="{1F9C4842-7E2D-40E4-8810-9F7B34D54D76}"/>
+    <hyperlink ref="H26" r:id="rId15" location="Werkstoff%3Du(85eb5967-f719-44cc-a7f3-84339b5839ac)%3Bd1%3Dc(25)%3Bd3%3Du(0c49c7b3-a2d5-4127-b6ac-792d414b1606)%3BForm%3Du(c0aa885f-8ea8-4010-abd2-06a95d4f35f0)" xr:uid="{D6B2EA74-8003-4424-A06E-78E36D093C76}"/>
+    <hyperlink ref="H32" r:id="rId16" xr:uid="{53E8A669-3EB3-4259-A86D-EAE251CED179}"/>
+    <hyperlink ref="H21" r:id="rId17" xr:uid="{C24409C7-1B7A-4386-B792-63EA1927E97A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -8380,7 +8258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C95DF24-9A3F-4553-BF69-26B88B2716A4}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -8391,54 +8269,54 @@
     <col min="2" max="2" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>361</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>391</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>362</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>363</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>364</v>
-      </c>
-      <c r="I1" s="38" t="s">
-        <v>365</v>
+      <c r="A1" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="100.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -8451,16 +8329,16 @@
         <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="G3" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>161</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>51</v>
@@ -8477,19 +8355,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>239</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>238</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="G4" s="35" t="s">
-        <v>241</v>
+        <v>81</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>51</v>
@@ -8508,17 +8386,17 @@
       <c r="C5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="35" t="s">
-        <v>256</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>243</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>257</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>258</v>
+      <c r="D5" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>51</v>
@@ -8537,17 +8415,17 @@
       <c r="C6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="35" t="s">
-        <v>255</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>244</v>
-      </c>
-      <c r="F6" s="35" t="s">
+      <c r="D6" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="G6" s="35" t="s">
-        <v>259</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>51</v>
@@ -8564,19 +8442,19 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>245</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="G7" s="35" t="s">
-        <v>260</v>
+        <v>247</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>51</v>
@@ -8596,16 +8474,16 @@
         <v>60</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="E8" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="F8" s="33" t="s">
-        <v>250</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>261</v>
+      <c r="E8" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>256</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>51</v>
@@ -8625,16 +8503,16 @@
         <v>59</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>247</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>249</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>262</v>
+        <v>243</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>51</v>
@@ -8644,17 +8522,17 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="55"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
     </row>
     <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -8667,16 +8545,16 @@
         <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="F11" s="42" t="s">
-        <v>265</v>
+        <v>259</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>260</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>51</v>
@@ -8696,16 +8574,16 @@
         <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="E12" s="33" t="s">
-        <v>266</v>
-      </c>
-      <c r="F12" s="42" t="s">
-        <v>274</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>51</v>
@@ -8721,20 +8599,20 @@
       <c r="B13" s="1">
         <v>4</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>270</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>267</v>
-      </c>
-      <c r="F13" s="42" t="s">
-        <v>273</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>277</v>
+      <c r="D13" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>51</v>
@@ -8751,19 +8629,19 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>272</v>
+        <v>266</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>51</v>
@@ -8773,108 +8651,108 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="55"/>
-    </row>
-    <row r="16" spans="1:9" s="14" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
+    </row>
+    <row r="16" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
         <v>1</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="F16" s="42" t="s">
-        <v>280</v>
-      </c>
-      <c r="G16" s="12"/>
+      <c r="D16" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G16" s="1"/>
       <c r="H16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="4">
         <v>6.14</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="55"/>
-    </row>
-    <row r="18" spans="1:9" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A17" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="31"/>
+    </row>
+    <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
         <v>1</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="1">
         <v>28</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="F18" s="42" t="s">
-        <v>283</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>293</v>
+      <c r="C18" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="4">
         <v>7.33</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="30">
+      <c r="A19" s="10">
         <v>1</v>
       </c>
-      <c r="B19" s="39">
+      <c r="B19" s="1">
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>286</v>
+        <v>290</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>292</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>0</v>
@@ -8890,20 +8768,20 @@
       <c r="B20" s="1">
         <v>2</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="D20" s="15" t="s">
+      <c r="C20" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>288</v>
+      <c r="D20" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>291</v>
+        <v>285</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>286</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>0</v>
@@ -8929,44 +8807,44 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="17"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="11"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="17"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="17"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="2"/>
@@ -9011,6 +8889,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AAB6B33AAADB4749B5B2EC20A535BB07" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cdc2803df0fb6ee94ea51a86a1ac5257">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="c035dcc5-7e05-44d6-8b62-8e13ee76956a" xmlns:ns4="3c154e5e-eb98-4d8e-85bb-17313b0ff9ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bacface54d10aab7e67a61770c43dbe2" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9244,15 +9131,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -9263,6 +9141,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BA8B08B-0469-4FB4-9569-1E0C636A2DDB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E048F32-FA24-43BF-92BF-83F9D5FCD2DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9278,14 +9164,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BA8B08B-0469-4FB4-9569-1E0C636A2DDB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>